<commit_message>
Dec 17th 6th Commit
</commit_message>
<xml_diff>
--- a/KPI_ACTION_TRACKER.xlsx
+++ b/KPI_ACTION_TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\usat-dfs\INTL\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3997381E-8953-4950-8354-BBC0EC5A71B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C39AA-6D44-42E2-AA4F-6C29E088F62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,10 +19,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -86,23 +95,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>What(Action Items)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>POT% is not meeting 100% even though we are on target(over 80%).</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Nizam, Hakimi &amp; Hanis</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Who(Responsible)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>When(Due date)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -194,14 +191,6 @@
   </si>
   <si>
     <t>Appzen Configuration setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Have to discuss further with IT representative
-</t>
-  </si>
-  <si>
-    <t>1. Need discussion with Yamazaki-san and other party to solve user's question
-2. Send VoC survey after providing answers to users</t>
   </si>
   <si>
     <t>C &amp; B analysis - Relocation fees process alignment</t>
@@ -354,6 +343,23 @@
   <si>
     <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - by end of Dec. 2021
 2. Giving consistent guide of the change to users via email and messages whenever contacted -end of Jan. 2022</t>
+  </si>
+  <si>
+    <t>1. Need discussion with Yamazaki-san and other party to solve user's question by end of December
+2. Send one VoC survey after providing answers to users by end of January 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Have to discuss further with IT representative by mid of January
+</t>
+  </si>
+  <si>
+    <t>What_Action_Items</t>
+  </si>
+  <si>
+    <t>Who_Responsible</t>
+  </si>
+  <si>
+    <t>When_Due_date</t>
   </si>
 </sst>
 </file>
@@ -772,7 +778,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -790,16 +796,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -816,16 +822,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>8</v>
@@ -836,19 +842,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -859,17 +865,17 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -880,20 +886,20 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.5">
@@ -901,17 +907,17 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>8</v>
@@ -922,38 +928,38 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.5">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>8</v>
@@ -961,22 +967,22 @@
     </row>
     <row r="9" spans="1:7" ht="87">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>8</v>
@@ -984,22 +990,22 @@
     </row>
     <row r="10" spans="1:7" ht="217.5">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>8</v>
@@ -1007,22 +1013,22 @@
     </row>
     <row r="11" spans="1:7" ht="159.5">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
@@ -1030,20 +1036,20 @@
     </row>
     <row r="12" spans="1:7" ht="29">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
@@ -1051,22 +1057,22 @@
     </row>
     <row r="13" spans="1:7" ht="72.5">
       <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>8</v>
@@ -1074,22 +1080,22 @@
     </row>
     <row r="14" spans="1:7" ht="58">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -1097,20 +1103,20 @@
     </row>
     <row r="15" spans="1:7" ht="29">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>8</v>
@@ -1118,20 +1124,20 @@
     </row>
     <row r="16" spans="1:7" ht="29">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>8</v>
@@ -1139,20 +1145,20 @@
     </row>
     <row r="17" spans="1:7" ht="29">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>8</v>
@@ -1160,20 +1166,20 @@
     </row>
     <row r="18" spans="1:7" ht="29">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>8</v>
@@ -1181,20 +1187,20 @@
     </row>
     <row r="19" spans="1:7" ht="43.5">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>8</v>
@@ -1202,20 +1208,20 @@
     </row>
     <row r="20" spans="1:7" ht="43.5">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>8</v>
@@ -1223,41 +1229,41 @@
     </row>
     <row r="21" spans="1:7" ht="29">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>8</v>
@@ -1265,20 +1271,20 @@
     </row>
     <row r="23" spans="1:7" ht="29">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>8</v>
@@ -1286,20 +1292,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>8</v>
@@ -1307,22 +1313,22 @@
     </row>
     <row r="25" spans="1:7" ht="39" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>8</v>
@@ -1330,22 +1336,22 @@
     </row>
     <row r="26" spans="1:7" ht="35.5" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>8</v>
@@ -1353,20 +1359,20 @@
     </row>
     <row r="27" spans="1:7" ht="58">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Dec 17th Commit v6
</commit_message>
<xml_diff>
--- a/KPI_ACTION_TRACKER.xlsx
+++ b/KPI_ACTION_TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\UPLOAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C39AA-6D44-42E2-AA4F-6C29E088F62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C927D832-5BDF-450A-B10F-7C0A56ABC33B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="status" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
   <si>
     <t>Why</t>
     <phoneticPr fontId="2"/>
@@ -213,10 +213,6 @@
   </si>
   <si>
     <t>Revised T&amp;E Thresholds Guide to users in KR12</t>
-  </si>
-  <si>
-    <t>1. Notification email with explanation on changes in amount thresholds to be sent out within Dec. 2021
-2. Live session on the changes to be conducted in 6 Jan. 2022</t>
   </si>
   <si>
     <t>1. Translation to be completed upon receiving access to the confidential document form Global team within Dec. 2021</t>
@@ -259,10 +255,6 @@
     <t>Since Nizam is leaving leave Alcon. All the task will be transfer to Hakimi and Hanis</t>
   </si>
   <si>
-    <t>1. To expediate KT, KT is currently being held everyday. 
-2. KT is expected to be completed by end of this year.</t>
-  </si>
-  <si>
     <t>1. Drafting all the related Tasks.</t>
   </si>
   <si>
@@ -341,25 +333,49 @@
     <t>Query submission mode change to FNOW guidance to all users in KR</t>
   </si>
   <si>
-    <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - by end of Dec. 2021
+    <t>What_Action_Items</t>
+  </si>
+  <si>
+    <t>Who_Responsible</t>
+  </si>
+  <si>
+    <t>When_Due_date</t>
+  </si>
+  <si>
+    <t>1. Ticket raised, waiting reply from IT team on customer's issue: VIM approval history. 
+2. Translating survey and preparing survey for customers by 2nd week of January 2022
+3.. Send one VoC survey after providing answers to users by end of January 2022
+4. To understand Yamasaki's task to prevent invoices from being neglected by end of December</t>
+  </si>
+  <si>
+    <t>VIM Insight Page-FNOW Link Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some users use wrong link to access SNOW. Instead of SNOW prod, they went to SNOW stage </t>
+  </si>
+  <si>
+    <t>Hakimi</t>
+  </si>
+  <si>
+    <t>1. To check and provide correct links for SNOW in the insight page (Jan 1st week)
+2. To check FNOW template link (Jan 1st week)</t>
+  </si>
+  <si>
+    <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - DONE 17 Dec.2021
 2. Giving consistent guide of the change to users via email and messages whenever contacted -end of Jan. 2022</t>
   </si>
   <si>
-    <t>1. Need discussion with Yamazaki-san and other party to solve user's question by end of December
-2. Send one VoC survey after providing answers to users by end of January 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Have to discuss further with IT representative by mid of January
+    <t>1. Notification email with explanation on changes in amount thresholds to be sent out within Dec. 2021-DONE 17 Dec. 2021
+2. Live session on the changes to be conducted in 6 Jan. 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Target at collecting 1,000 Knowledge idea as a team
+2. Have to discuss further with IT representative by mid of January
 </t>
   </si>
   <si>
-    <t>What_Action_Items</t>
-  </si>
-  <si>
-    <t>Who_Responsible</t>
-  </si>
-  <si>
-    <t>When_Due_date</t>
+    <t>1. To expediate KT, KT is currently being held everyday. 
+2. KT is expected to be completed by end of Feb, 2022.</t>
   </si>
 </sst>
 </file>
@@ -441,7 +457,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -456,6 +472,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -775,17 +800,17 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.90625" customWidth="1"/>
     <col min="2" max="2" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="5" width="15.90625" customWidth="1"/>
     <col min="6" max="6" width="70.81640625" customWidth="1"/>
     <col min="7" max="7" width="15.90625" customWidth="1"/>
@@ -796,16 +821,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -854,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -917,7 +942,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>8</v>
@@ -938,13 +963,13 @@
         <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.5">
+    <row r="8" spans="1:7" ht="101.5">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -970,19 +995,19 @@
         <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>8</v>
@@ -996,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>
@@ -1005,7 +1030,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>8</v>
@@ -1019,7 +1044,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>32</v>
@@ -1028,13 +1053,13 @@
         <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29">
+    <row r="12" spans="1:7" ht="43.5">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1049,7 +1074,7 @@
         <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
@@ -1063,7 +1088,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>34</v>
@@ -1072,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>8</v>
@@ -1086,7 +1111,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
@@ -1095,7 +1120,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -1116,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>8</v>
@@ -1137,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>8</v>
@@ -1158,7 +1183,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>8</v>
@@ -1179,7 +1204,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>8</v>
@@ -1200,7 +1225,7 @@
         <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>8</v>
@@ -1221,7 +1246,7 @@
         <v>27</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>8</v>
@@ -1232,7 +1257,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
@@ -1242,7 +1267,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>48</v>
@@ -1253,7 +1278,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
@@ -1263,7 +1288,7 @@
         <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>8</v>
@@ -1274,7 +1299,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
@@ -1284,7 +1309,7 @@
         <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>8</v>
@@ -1295,17 +1320,17 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>8</v>
@@ -1316,19 +1341,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>8</v>
@@ -1339,19 +1364,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="F26" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>8</v>
@@ -1362,7 +1387,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
@@ -1372,14 +1397,46 @@
         <v>44</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="28" spans="1:7" ht="58">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G23" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1431,7 +1488,6 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
     <customPr name="_pios_id" r:id="rId2"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit Dec 27th v1
</commit_message>
<xml_diff>
--- a/KPI_ACTION_TRACKER.xlsx
+++ b/KPI_ACTION_TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\UPLOAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C927D832-5BDF-450A-B10F-7C0A56ABC33B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91C6334-58AD-47AD-BEA9-9532B3986527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,28 +17,19 @@
     <sheet name="status" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$33</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="123">
   <si>
     <t>Why</t>
     <phoneticPr fontId="2"/>
@@ -103,11 +94,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>1. Consistency checking between payment term and actual invoice manually
-2. Identify the reason of deviated invoices whether it is due to system related only</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>DAT(Duplicate Audit Tool)</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -197,9 +183,6 @@
   </si>
   <si>
     <t>Jan, 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. To align with HR team and Payroll team on the process of transportation fares for family visitation </t>
   </si>
   <si>
     <t>C &amp; B analysis - OT-related costs process alignment</t>
@@ -216,9 +199,6 @@
   </si>
   <si>
     <t>1. Translation to be completed upon receiving access to the confidential document form Global team within Dec. 2021</t>
-  </si>
-  <si>
-    <t>1. Revision on Local Addendum based on the new thresholds and revised Global policy</t>
   </si>
   <si>
     <t>1. Meeting with GPO on confirmation of congifuration setting chage within Dec. 2021
@@ -241,9 +221,6 @@
 5. After January %POT Analysis, if the additional Payment cycle is required, R2P will work with TCM task owner closely in order to prevent any service quality disruption (Feb 2022) </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Revision on Local Addendum based on the new thresholds and revised Global policy </t>
-  </si>
-  <si>
     <t>Since Asano san will be transferred to another department. All the task will be transfer to AGSKL team</t>
   </si>
   <si>
@@ -255,6 +232,10 @@
     <t>Since Nizam is leaving leave Alcon. All the task will be transfer to Hakimi and Hanis</t>
   </si>
   <si>
+    <t>1. To expediate KT, KT is currently being held everyday. 
+2. KT is expected to be completed by end of this year.</t>
+  </si>
+  <si>
     <t>1. Drafting all the related Tasks.</t>
   </si>
   <si>
@@ -262,12 +243,6 @@
   </si>
   <si>
     <t>Action - Required team to update the excel for training material which required to be updates and provide updates by 21st Dec</t>
-  </si>
-  <si>
-    <t>Update of Concur Approver Training &amp; related materials on T&amp;E InSight Page</t>
-  </si>
-  <si>
-    <t>Action - Required team to update the excel for training material which required to be updates by 21st Dec</t>
   </si>
   <si>
     <t>KPI for T&amp;E Compliance Rate are below 85%</t>
@@ -293,28 +268,15 @@
 3. Decide whether we implement new process or not based on our parallel run</t>
   </si>
   <si>
-    <t>1. Design a separate Rejection Analysis to identify main contributor of rejection in Concur (Jun 2021)
-2. Build an action plan to achieve KPI target of 85% Compliance rate before end of 2021. (Nov 2021)
-3. Create a Newsletter to touch on monthly Top 3 Rejection reason and any other important notification for all Japan Business User (Dec 2021)
-4. Create other separate email notification to targeted users regarding specific rejection reason in order to increase effectiveness as a follow up action. (Dec 2021)
-5. Conduct a direct session in Jan 2022 with users who committed the rejection reason repeatedly since Aug 2021 (in progress)</t>
-  </si>
-  <si>
     <t>Downpayment Case Study</t>
   </si>
   <si>
     <t xml:space="preserve">Syahmi  </t>
   </si>
   <si>
-    <t>To update manual on several special case for downpayment occured througout year 2021</t>
-  </si>
-  <si>
     <t>Donation</t>
   </si>
   <si>
-    <t>To update SOP for yearly task donation which is incompletely transfered from Iida-san in March 2021</t>
-  </si>
-  <si>
     <t>The task is performed rarely once in year end and new year, thus need to have a clear manual for future new joiner</t>
   </si>
   <si>
@@ -327,12 +289,13 @@
     <t>Feb, 2022</t>
   </si>
   <si>
-    <t>To go through payment KT by Nizam with Hanis for payment task to refresh on the opration flow.</t>
-  </si>
-  <si>
     <t>Query submission mode change to FNOW guidance to all users in KR</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Have to discuss further with IT representative by mid of January
+</t>
+  </si>
+  <si>
     <t>What_Action_Items</t>
   </si>
   <si>
@@ -342,40 +305,158 @@
     <t>When_Due_date</t>
   </si>
   <si>
-    <t>1. Ticket raised, waiting reply from IT team on customer's issue: VIM approval history. 
+    <t>VIM Insight Page-FNOW Link Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some users use wrong link to access SNOW. Instead of SNOW prod, they went to SNOW stage </t>
+  </si>
+  <si>
+    <t>Hakimi</t>
+  </si>
+  <si>
+    <t>1. To check and provide correct links for SNOW in the insight page (Jan 1st week)
+2. To check FNOW template link (Jan 1st week)</t>
+  </si>
+  <si>
+    <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - DONE 17 Dec.2021
+2. Giving consistent guide of the change to users via email and messages whenever contacted -end of Jan. 2022</t>
+  </si>
+  <si>
+    <t>1. Notification email with explanation on changes in amount thresholds to be sent out within Dec. 2021-DONE 17 Dec. 2021
+2. Live session on the changes to be conducted in 6 Jan. 2022</t>
+  </si>
+  <si>
+    <t>Kota</t>
+  </si>
+  <si>
+    <t>1. To check year end closing calendar updated by Syahmi and identify critical items along with due dates (Dec 22, 2021)
+2. Arrange the quick session to explain year end closing calenders along with action items (Dec 23, 2021)</t>
+  </si>
+  <si>
+    <t>Global and Japan WD calendar is not aligned for the year end closing.</t>
+  </si>
+  <si>
+    <t>2022 Payment calendar</t>
+  </si>
+  <si>
+    <t>Payment calendar has not yet been created before, so the approvers have to handle payment approveal on ad-hoc basis.</t>
+  </si>
+  <si>
+    <t>1. To check 2022 payment calendar updated by Nizam and identify if there is any discrepancy between payment run date and our assumption (Dec 22, 2021)
+2. Arrange the quick session to explain 2022 payment calendar (Dec 23, 2021)</t>
+  </si>
+  <si>
+    <t>KPI T&amp;E update</t>
+  </si>
+  <si>
+    <t>T&amp;E dashboard has been updated in global tableau platform, but it takes some time to take a snapshot of each KPI graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Build a python programming utilizing scraping technique to automatically scrape the dashboard (Dec 23, 2021)
+2. Automate copy and paste process of screenshots into deck (Dec 23, 2021) </t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>1. IT team reverted to FRA team. Discuss with Nicholas, Nicholas to deliver feedback
 2. Translating survey and preparing survey for customers by 2nd week of January 2022
 3.. Send one VoC survey after providing answers to users by end of January 2022
 4. To understand Yamasaki's task to prevent invoices from being neglected by end of December</t>
   </si>
   <si>
-    <t>VIM Insight Page-FNOW Link Update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some users use wrong link to access SNOW. Instead of SNOW prod, they went to SNOW stage </t>
-  </si>
-  <si>
-    <t>Hakimi</t>
-  </si>
-  <si>
-    <t>1. To check and provide correct links for SNOW in the insight page (Jan 1st week)
-2. To check FNOW template link (Jan 1st week)</t>
-  </si>
-  <si>
-    <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - DONE 17 Dec.2021
-2. Giving consistent guide of the change to users via email and messages whenever contacted -end of Jan. 2022</t>
-  </si>
-  <si>
-    <t>1. Notification email with explanation on changes in amount thresholds to be sent out within Dec. 2021-DONE 17 Dec. 2021
-2. Live session on the changes to be conducted in 6 Jan. 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Target at collecting 1,000 Knowledge idea as a team
-2. Have to discuss further with IT representative by mid of January
+    <t>FNOW Breached Ticket Analysis</t>
+  </si>
+  <si>
+    <t>1. To provide simple workflow for breached ticket analysis  Feb 25, 2021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. To align with HR team and Payroll team on the process of transportation fares for family visitation - to arrange a meeting in Jan. </t>
+  </si>
+  <si>
+    <t>1. Translation to be completed upon receiving access to the confidential document form Global team within Dec. 2021- to be completed by 23 Dec. 2021</t>
+  </si>
+  <si>
+    <t>1. Revision on Local Addendum based on the new thresholds and revised Global policy - to be completed by 23 Dec. 2021</t>
+  </si>
+  <si>
+    <t>1. Meeting with GPO on confirmation of congifuration setting chage within Dec. 2021-DONE on 21 Dec. 2021
+2. Request the change to Appzen team and apply the new configuration - by end of Dec. 2021</t>
+  </si>
+  <si>
+    <t>To update manual on several special case for downpayment occured througout year 2021 (In progress)</t>
+  </si>
+  <si>
+    <t>Dec, 2022</t>
+  </si>
+  <si>
+    <t>1. To update SOP for yearly task donation which is incompletely transfered from Iida-san in March 2021 (end of Dec)</t>
+  </si>
+  <si>
+    <t>1. To go through payment KT by Nizam with Hanis for payment task to refresh on the opration flow (end of Dec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate Audit Tools </t>
+  </si>
+  <si>
+    <t>Syahmi and Nadzrin</t>
+  </si>
+  <si>
+    <t>1. Knowledge sharing on new DAT with team</t>
+  </si>
+  <si>
+    <t>Automated Posting : T&amp;E accrual Global Enhancement</t>
+  </si>
+  <si>
+    <t>The system to go live on Jannuary 2022</t>
+  </si>
+  <si>
+    <t>1. Knowledge sharing on new project of Automated Posting : T&amp;E accrual Global Enhancement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an alternative way to double confirm current practice / to replace current practice which consume much time </t>
+  </si>
+  <si>
+    <t>1. Revision on Local Addendum based on the new thresholds and revised Global policy by 24 Dec 2021</t>
+  </si>
+  <si>
+    <t>1. Design a separate Rejection Analysis to identify main contributor of rejection in Concur (Done on Jun 2021)
+2. Build an action plan to achieve KPI target of 85% Compliance rate before end of 2021. (Done on Nov 2021)
+3. Create a Newsletter to touch on monthly Top 3 Rejection reason and any other important notification for all Japan Business User (Done on Dec 2021)
+4. Create other separate email notification to targeted users regarding specific rejection reason in order to increase effectiveness as a follow up action. (Done on Dec 2021)
+5. Conduct a direct session in Jan 2022 with users who committed the rejection reason repeatedly since Aug 2021 (invitation will be sent by 14 Jan 2021, session by 21 Jan 2021)</t>
+  </si>
+  <si>
+    <t>Year End Schedule update</t>
+  </si>
+  <si>
+    <t>Hiring status</t>
+  </si>
+  <si>
+    <t>Replecement of Aiqi and Nizam</t>
+  </si>
+  <si>
+    <t>Sharil (replacement of Aiqi) will be joining us on Feb3, 2022. He will be signing our job offer letter.
+Nurulain(replacement of Nizam) will be joining us on Jan 4th, 2022. Job offer letter will be signed off by her after HR manager e-signs it.</t>
+  </si>
+  <si>
+    <t>Paperless Project</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to Law Concerning Preservation of National Tax Records in Electronic Form, Concur process change will be required. </t>
+  </si>
+  <si>
+    <t>1. Consistency checking between payment term and actual invoice manually (Dec 31, 2021)
+2. Identify the reason of deviated invoices whether it is due to system related only (Jan 14, 2022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Appzen current configuration setting revisit Jan 7, 2022
+2. Public transporation configuration as a reference point Jan 7, 2022
+3. Feasibility study whether Appzen can flag it as medium or low risk if the users attach only credit card statement
 </t>
-  </si>
-  <si>
-    <t>1. To expediate KT, KT is currently being held everyday. 
-2. KT is expected to be completed by end of Feb, 2022.</t>
   </si>
 </sst>
 </file>
@@ -429,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -448,6 +529,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -457,7 +556,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -473,14 +572,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -800,19 +917,20 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.90625" customWidth="1"/>
     <col min="2" max="2" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="70.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="114" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -821,16 +939,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -839,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.5">
+    <row r="2" spans="1:7" ht="58">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -856,51 +974,51 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="72.5">
+    <row r="3" spans="1:7" ht="159.5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -911,38 +1029,38 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>8</v>
@@ -953,174 +1071,174 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="101.5">
+    <row r="8" spans="1:7" ht="58">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="58">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409.5">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="87">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="217.5">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="116">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="159.5">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.5">
+    <row r="12" spans="1:7" ht="29">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="72.5">
+    <row r="13" spans="1:7" ht="130.5">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="116">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="58">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -1128,315 +1246,583 @@
     </row>
     <row r="15" spans="1:7" ht="29">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.5">
+    <row r="19" spans="1:8" ht="29">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.5">
+    <row r="20" spans="1:8" ht="29">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="29">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="29">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="29">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="29">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="29">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>64</v>
+        <v>36</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8" ht="39" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="35.5" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="29">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="116">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="87">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="159.5">
+      <c r="A29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="174">
+      <c r="A30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2"/>
+      <c r="B31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="39" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="35.5" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="58">
-      <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="58">
-      <c r="A28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="5"/>
+      <c r="F31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="188.5">
+      <c r="A32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="58">
+      <c r="A33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="43.5">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="130.5">
+      <c r="A35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G33" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1444,6 +1830,18 @@
     <customPr name="_pios_id" r:id="rId2"/>
     <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>status!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G48</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1488,6 +1886,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
     <customPr name="_pios_id" r:id="rId2"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit Dec 27th v2
</commit_message>
<xml_diff>
--- a/KPI_ACTION_TRACKER.xlsx
+++ b/KPI_ACTION_TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAEDAKO1\OneDrive - Alcon\DESKTOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91C6334-58AD-47AD-BEA9-9532B3986527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA4A4B-2C2C-4A24-84ED-323E8F71AA99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="124">
   <si>
     <t>Why</t>
     <phoneticPr fontId="2"/>
@@ -453,9 +453,12 @@
 2. Identify the reason of deviated invoices whether it is due to system related only (Jan 14, 2022)</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Appzen current configuration setting revisit Jan 7, 2022
-2. Public transporation configuration as a reference point Jan 7, 2022
-3. Feasibility study whether Appzen can flag it as medium or low risk if the users attach only credit card statement
+    <t>Overdue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Appzen current configuration setting revisit (Jan 7, 2022)
+2. Public transporation configuration as a reference point (Jan 7, 2022)
+3. Feasibility study whether Appzen can flag it as medium or low risk if the users attach only credit card statement (Jan 7, 2022)
 </t>
   </si>
 </sst>
@@ -919,8 +922,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -980,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="159.5">
+    <row r="3" spans="1:7" ht="101.5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="409.5">
+    <row r="10" spans="1:7" ht="290">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="130.5">
+    <row r="13" spans="1:7" ht="87">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="116">
+    <row r="14" spans="1:7" ht="72.5">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="116">
+    <row r="27" spans="1:8" ht="87">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="87">
+    <row r="28" spans="1:8" ht="58">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -1543,10 +1546,10 @@
         <v>85</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="159.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="101.5">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
@@ -1566,10 +1569,10 @@
         <v>89</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="174">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="101.5">
       <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>92</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1612,7 +1615,7 @@
       </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="188.5">
+    <row r="32" spans="1:8" ht="101.5">
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="58">
+    <row r="33" spans="1:7" ht="43.5">
       <c r="A33" s="2" t="s">
         <v>23</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>43</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>119</v>

</xml_diff>